<commit_message>
Test Data Updated to match passwords correctly
</commit_message>
<xml_diff>
--- a/src/test/java/com/automation/mypreparation/testdata/TestData.xlsx
+++ b/src/test/java/com/automation/mypreparation/testdata/TestData.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E613D318-65B9-4DB1-9C30-10657030796C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14790" windowHeight="6345"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="14820" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
   <oleSize ref="A1:M19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>UserName</t>
   </si>
@@ -35,9 +36,6 @@
   </si>
   <si>
     <t>yuvi.subu2@yopmail.com</t>
-  </si>
-  <si>
-    <t>Welcome@12</t>
   </si>
   <si>
     <t>Include</t>
@@ -55,8 +53,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +104,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -152,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -184,9 +190,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,6 +242,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -393,20 +435,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,10 +456,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -428,18 +470,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -452,49 +494,49 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
-    <hyperlink ref="B4" r:id="rId6"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -503,12 +545,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
latest change after windows recovery
</commit_message>
<xml_diff>
--- a/src/test/java/com/automation/mypreparation/testdata/TestData.xlsx
+++ b/src/test/java/com/automation/mypreparation/testdata/TestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5234007D-DF6F-47F7-A46B-9369F90784CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5AED50A9-DEEF-4EA7-9C1E-EBFC2D9A7CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="14850" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="14880" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>